<commit_message>
Comentarios, casos de prueba
Se añade la tabla pivote, y los comentarios de creación.
</commit_message>
<xml_diff>
--- a/Documentación/Casos de prueba.xlsx
+++ b/Documentación/Casos de prueba.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr hidePivotFieldList="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ED-Veneno\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Veneno Game - Casos" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId1"/>
+    <sheet name="Veneno Game - Casos" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Certificado">'Veneno Game - Casos'!$G$4:$G$6</definedName>
     <definedName name="Estado">'Veneno Game - Casos'!$G$4:$G$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <pivotCaches>
+    <pivotCache cacheId="17" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="95">
   <si>
     <t>Casos de prueba</t>
   </si>
@@ -301,13 +305,25 @@
   </si>
   <si>
     <t>Se valida el boton de juego.</t>
+  </si>
+  <si>
+    <t>Total general</t>
+  </si>
+  <si>
+    <t>Etiquetas de fila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuenta de Id </t>
+  </si>
+  <si>
+    <t>Tabla Pivote</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,7 +332,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -324,7 +339,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -340,7 +364,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -357,12 +381,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -372,21 +396,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b/>
+        <i val="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -418,958 +473,403 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-ES"/>
-              <a:t>Analisis</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-ES" baseline="0"/>
-              <a:t> de Caso de P</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-ES" baseline="0"/>
-              <a:t>rueba.</a:t>
-            </a:r>
-            <a:endParaRPr lang="es-ES"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.40008168479749101"/>
-          <c:y val="2.7777777777777776E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="1"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="2"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-    </c:pivotFmts>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Total</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="3"/>
-              <c:pt idx="0">
-                <c:v>Certificado</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Pendiente</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Con Error</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="3"/>
-              <c:pt idx="0">
-                <c:v>1</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>47</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>2</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6EDD-42CA-9ED1-2F8584AFAC60}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="802981199"/>
-        <c:axId val="802980367"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="802981199"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="802980367"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="802980367"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="802981199"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:extLst/>
-</c:chartSpace>
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="15" refreshedDate="42844.490463310183" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="50">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Tabla1"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Id " numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="50"/>
+    </cacheField>
+    <cacheField name="Descripción" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Resultado esperado" numFmtId="0">
+      <sharedItems containsBlank="1" longText="1"/>
+    </cacheField>
+    <cacheField name="Estado" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Certificado"/>
+        <s v="Pendiente"/>
+        <s v="Con Error"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="50">
+  <r>
+    <n v="1"/>
+    <s v="Al iniciar el juego se abre correctamente el socket."/>
+    <s v="Se ejecute background en un proceso de Windows."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="Al precionar el ejecutable se ejecuta el apache y las dependencias."/>
+    <s v="Al iniciar se ejecute como aplicación secundaria el modulo apache y sus dependencias, sin que el usuario lo observe."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <s v="Al abrir se abre correctamente el index e inicia la animacion principal."/>
+    <s v="Al iniciar se abre correctamente el explorador por defecto y se inicia la animacion principal."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <s v="En todas las pantallas de juego existe el enlace al manual de usuario. "/>
+    <s v="Cada pantalla con un enlace al manual de usuario, y que este este correctamente enlazado."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <s v="En todas las pantallas de juego existe un enlace a atraz validando en los casos en los que no pueda ir, como al inciar la consola de juego. "/>
+    <s v="Enlaces de atraz correctamente validados alas pantallas correspondientes"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <s v="El drag and drop del juego."/>
+    <s v="La animacion del drag and drop funciona con las cartas y de desactiva cuando se finaliza."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <s v="Se valida la carta con la UI en el caldero y verifica que la carta pueda o no colocarse en el caldero"/>
+    <s v="Muestra una alerta que impide que se coloque la carta cuando la carta no esta en el caldero correcto. "/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <s v="Se valida el boton de juego."/>
+    <s v="Se valida la activacion y una alerta cuando se intente jugar sin mover la carta en el caldero."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <s v="Asignar la cantidad de jugadores en uno."/>
+    <s v="No se puede crear solo un jugador, el mínimo son dos."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <s v="Asignar la cantidad de jugadores en dos."/>
+    <s v="La cantidad es aceptada correctamente."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <s v="Asignar la cantidad de jugadores en siete."/>
+    <s v="No es posible, el máximo son seis jugadores."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <s v="No digita el nombre del jugador al crearlo."/>
+    <s v="Se le asigna como nombre &quot;Jugador n&quot;, donde n es el número del jugador."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <s v="Digita un nombre al jugador al crearlo."/>
+    <s v="Se le asigna el string digitado como nombre al guardar el jugador en la lista."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <s v="Se crean seis jugadores, se les asigna un nombre a cada uno."/>
+    <s v="La lista de jugadores debe contener 6 jugadores, cada uno con el nombre asignado, y un id que indica el orden en que fueron creados."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <s v="Busca un jugador según su posición en la lista (la posición existe)."/>
+    <s v="La lista devuelve el objeto jugador en esa posición."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <s v="Busca un jugador según su posición en la lista (la posición no existe)."/>
+    <s v="La lista devuelve un mensaje de advertencia según sea el caso, la posición no es válida o la lista está vacía."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <s v="Busca la baraja de cartas en mano de un jugador en específico."/>
+    <s v="Devuelve la baraja  de cartas en mano, o un mensaje de advertencia en caso de que esta esté vacía."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <s v="Busca la baraja de cartas  comidas de un jugador en específico."/>
+    <s v="Devuelve la baraja  de cartas comidas, o un mensaje de advertencia en caso de que esta esté vacía."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <s v="Busca la baraja de cartas veneno de un jugador en específico."/>
+    <s v="Devuelve la baraja  de cartas veneno, o un mensaje de advertencia en caso de que esta esté vacía."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="20"/>
+    <s v="Llama a la opción barajar antes de empezar la ronda."/>
+    <s v="Se reparte una cantidad de cartas cada jugador según la cantidad de jugadores activos, estas cartas son repartidas de manera aleatoria."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="21"/>
+    <s v="Después de barajar  se consulta el pozo para repartir."/>
+    <s v="Devuelve el pozo, este debe ser el pozo original, menos las cartas previamente repartidas."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <s v="Llama a la opción barajar, mientras algún jugador todavía tiene cartas."/>
+    <s v="Sólo se puede barajar cuando todos los jugadores no tengan ninguna carta en la mano."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="23"/>
+    <s v="Llama a la opción barajar (en el pozo no quedan suficientes cartas para repartir según las reglas)"/>
+    <s v="Se termina la ronda."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <s v="Se añade una carta (que no es veneno) a un caldero vacío."/>
+    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <s v="Se añade una carta (que no es veneno) a un caldero no vacío, pero que tiene la misma nomenclatura. El total del caldero es menor que trece."/>
+    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <s v="Se añade una carta (que no es veneno) a un caldero con diferente nomenclatura."/>
+    <s v="El sistema rechaza el movimiento."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <s v="Se añade una carta (que no es veneno) a un caldero. El total del caldero da más de trece."/>
+    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador. Al verificar el total, da mayor de lo establecido, por lo cual las cartas en el caldero se pasan a la baraja de cartas comidas por el jugador. Admás si entre estas existen cartas venenos estas se pasan a la baraja de cartas veneno del jugador."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <s v="Se añade una carta veneno a un caldero no vacío. El total del caldero es menor que trece."/>
+    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <s v="Se añade una carta veneno a un caldero vacío. El jugador tiene más cartas en la mano."/>
+    <s v="Se rechaza el movimiento."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="30"/>
+    <s v="Se añade una carta veneno a un caldero vacío. El jugador sólo tiene esa carta en la mano."/>
+    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="31"/>
+    <s v="Se añade una carta veneno a un caldero que contiene solamente cartas veneno.  El jugador sólo tiene esa carta en la mano."/>
+    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <s v="Se añade una carta veneno a un caldero que contiene solamente cartas veneno.  El jugador tiene más cartas en la mano."/>
+    <s v="El sistema rechaza el movimiento."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="33"/>
+    <s v="Se añade una carta veneno a un caldero. El total del caldero da más de trece."/>
+    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador. Al verificar el total, da mayor de lo establecido, por lo cual las cartas en el caldero se pasan a la baraja de cartas comidas por el jugador. Admás si entre estas existen cartas venenos estas se pasan a la baraja de cartas veneno del jugador."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="34"/>
+    <s v="Pasar de turno sin haber añadido a algún caldero. El jugador tiene cartas en la mano."/>
+    <s v="El sistema no permite continuar con el juego hasta que el jugador en el turno mueva la carta."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="35"/>
+    <s v="Pasar de turno sin haber añadido a algún caldero. El jugador no tiene cartas."/>
+    <s v="Se realiza automáticamente, al jugador que se queda sin cartas se le pasa el turno."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="36"/>
+    <s v="Llamar la función undo, empezar una ronda."/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="37"/>
+    <s v="Llamar la función undo, en medio de una ronda."/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="38"/>
+    <s v="Llamar la función undo al finalizar la ronda."/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <s v="Llamar la función redo, sin ahaber realizado un undo."/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="40"/>
+    <s v="Llamar la función redo, después de un undo."/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="41"/>
+    <s v="Llamar la función redo, después de un undo, y luego jugar un movimiento"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="42"/>
+    <s v="Llamar la función redo dos veces después de un undo."/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="43"/>
+    <s v="Llamar la función reset al empezar una ronda."/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="44"/>
+    <s v="Llamar la función reset en medio de una ronda."/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="45"/>
+    <s v="Llamar la función reset al finalizar una ronda."/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="46"/>
+    <s v="Se acaban las cartas en el pozo de repartir. Un jugador no tiene ninguna carta veneno."/>
+    <s v="Se acaba la ronda y dicho jugador sale del juego."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="47"/>
+    <s v="Se acaban las cartas en el pozo de repartir. Ningún jugador tiene cartas veneno."/>
+    <s v="Se acaba el juego."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="48"/>
+    <s v="Se acaban las cartas en el pozo de repartir. Todos los jugadores tienen la misma cantidad de cartas venenos."/>
+    <s v="Se acaba el juego."/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="49"/>
+    <s v="Se acaban las cartas en el pozo para repartir. Varios jugadores tienen la misma cantidad de venenos."/>
+    <s v="Se crea una neva ronda, y se sacan del juego los jugadores que tengan menor cantidad de venenos."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="50"/>
+    <s v="Se acaban las cartas en el pozo para repartir. Sólo quedan dos jugadores."/>
+    <s v="Se saca el jugador con menos cartas venenos, el otro es el perdedor."/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
 </file>
 
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>89647</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>44823</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>257735</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>121023</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B62:C66" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Cuenta de Id " fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B4:E54" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B4:E54" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="B4:E54"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Id " dataDxfId="4"/>
-    <tableColumn id="2" name="Descripción" dataDxfId="3"/>
-    <tableColumn id="3" name="Resultado esperado" dataDxfId="2"/>
-    <tableColumn id="4" name="Estado" dataDxfId="1"/>
+    <tableColumn id="1" name="Id " dataDxfId="6"/>
+    <tableColumn id="2" name="Descripción" dataDxfId="5"/>
+    <tableColumn id="3" name="Resultado esperado" dataDxfId="4"/>
+    <tableColumn id="4" name="Estado" dataDxfId="3"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1670,10 +1170,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G54"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="A3:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60:C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,7 +1201,7 @@
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2400,43 +1918,77 @@
         <v>7</v>
       </c>
     </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="10"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C62" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C66" s="9">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B60:C60"/>
   </mergeCells>
+  <conditionalFormatting sqref="E5:E54">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Con error">
+      <formula>NOT(ISERROR(SEARCH("Con error",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Pendiente">
+      <formula>NOT(ISERROR(SEARCH("Pendiente",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Certificado">
+      <formula>NOT(ISERROR(SEARCH("Certificado",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E53">
       <formula1>Estado</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{0D8DF6AD-002F-4C3D-BAF6-21FBBE4D6EDB}">
-            <xm:f>NOT(ISERROR(SEARCH($G$4,E5)))</xm:f>
-            <xm:f>$G$4</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E5:E53</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Casos de prueba, actualizado
</commit_message>
<xml_diff>
--- a/Documentación/Casos de prueba.xlsx
+++ b/Documentación/Casos de prueba.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ED-Veneno\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\Veneno\ED-Veneno\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja2" sheetId="3" r:id="rId1"/>
+    <sheet name="Tabla pivote" sheetId="5" r:id="rId1"/>
     <sheet name="Veneno Game - Casos" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -21,7 +21,8 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="17" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="10" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="100">
   <si>
     <t>Casos de prueba</t>
   </si>
@@ -82,9 +83,6 @@
     <t>Digita un nombre al jugador al crearlo.</t>
   </si>
   <si>
-    <t>Se le asigna como nombre "Jugador n", donde n es el número del jugador.</t>
-  </si>
-  <si>
     <t>Se le asigna el string digitado como nombre al guardar el jugador en la lista.</t>
   </si>
   <si>
@@ -100,12 +98,6 @@
     <t>Busca un jugador según su posición en la lista (la posición no existe).</t>
   </si>
   <si>
-    <t>La lista devuelve el objeto jugador en esa posición.</t>
-  </si>
-  <si>
-    <t>La lista devuelve un mensaje de advertencia según sea el caso, la posición no es válida o la lista está vacía.</t>
-  </si>
-  <si>
     <t>Busca la baraja de cartas en mano de un jugador en específico.</t>
   </si>
   <si>
@@ -199,39 +191,18 @@
     <t>Pasar de turno sin haber añadido a algún caldero. El jugador no tiene cartas.</t>
   </si>
   <si>
-    <t>Se realiza automáticamente, al jugador que se queda sin cartas se le pasa el turno.</t>
-  </si>
-  <si>
-    <t>Llamar la función undo, empezar una ronda.</t>
-  </si>
-  <si>
     <t>Llamar la función undo, en medio de una ronda.</t>
   </si>
   <si>
-    <t>Llamar la función undo al finalizar la ronda.</t>
-  </si>
-  <si>
-    <t>Llamar la función redo, sin ahaber realizado un undo.</t>
-  </si>
-  <si>
     <t>Llamar la función redo, después de un undo.</t>
   </si>
   <si>
-    <t>Llamar la función redo dos veces después de un undo.</t>
-  </si>
-  <si>
     <t>Llamar la función reset al empezar una ronda.</t>
   </si>
   <si>
     <t>Llamar la función reset en medio de una ronda.</t>
   </si>
   <si>
-    <t>Llamar la función reset al finalizar una ronda.</t>
-  </si>
-  <si>
-    <t>Llamar la función redo, después de un undo, y luego jugar un movimiento</t>
-  </si>
-  <si>
     <t>Se acaban las cartas en el pozo de repartir. Un jugador no tiene ninguna carta veneno.</t>
   </si>
   <si>
@@ -259,54 +230,21 @@
     <t>Se saca el jugador con menos cartas venenos, el otro es el perdedor.</t>
   </si>
   <si>
-    <t>Al precionar el ejecutable se ejecuta el apache y las dependencias.</t>
-  </si>
-  <si>
     <t>Al iniciar el juego se abre correctamente el socket.</t>
   </si>
   <si>
-    <t xml:space="preserve">En todas las pantallas de juego existe el enlace al manual de usuario. </t>
-  </si>
-  <si>
-    <t>Al abrir se abre correctamente el index e inicia la animacion principal.</t>
-  </si>
-  <si>
     <t>Se ejecute background en un proceso de Windows.</t>
   </si>
   <si>
-    <t>Al iniciar se ejecute como aplicación secundaria el modulo apache y sus dependencias, sin que el usuario lo observe.</t>
-  </si>
-  <si>
     <t>Al iniciar se abre correctamente el explorador por defecto y se inicia la animacion principal.</t>
   </si>
   <si>
     <t>Cada pantalla con un enlace al manual de usuario, y que este este correctamente enlazado.</t>
   </si>
   <si>
-    <t xml:space="preserve">En todas las pantallas de juego existe un enlace a atraz validando en los casos en los que no pueda ir, como al inciar la consola de juego. </t>
-  </si>
-  <si>
-    <t>Enlaces de atraz correctamente validados alas pantallas correspondientes</t>
-  </si>
-  <si>
-    <t>El drag and drop del juego.</t>
-  </si>
-  <si>
-    <t>La animacion del drag and drop funciona con las cartas y de desactiva cuando se finaliza.</t>
-  </si>
-  <si>
     <t>Se valida la carta con la UI en el caldero y verifica que la carta pueda o no colocarse en el caldero</t>
   </si>
   <si>
-    <t xml:space="preserve">Muestra una alerta que impide que se coloque la carta cuando la carta no esta en el caldero correcto. </t>
-  </si>
-  <si>
-    <t>Se valida la activacion y una alerta cuando se intente jugar sin mover la carta en el caldero.</t>
-  </si>
-  <si>
-    <t>Se valida el boton de juego.</t>
-  </si>
-  <si>
     <t>Total general</t>
   </si>
   <si>
@@ -316,7 +254,85 @@
     <t xml:space="preserve">Cuenta de Id </t>
   </si>
   <si>
-    <t>Tabla Pivote</t>
+    <t>Al iniciar se ejecute como aplicación secundaria el módulo apache y sus dependencias, sin que el usuario lo observe.</t>
+  </si>
+  <si>
+    <t>Al presionar el ejecutable se ejecuta el apache y las dependencias.</t>
+  </si>
+  <si>
+    <t>Iniciar el juego.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enlace al manual de usuario. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">En todas las pantallas de juego existe un enlace a atrás validando en los casos en los que no pueda ir, como al inciar la consola de juego. </t>
+  </si>
+  <si>
+    <t>Enlaces de atrás correctamente validados alas pantallas correspondientes</t>
+  </si>
+  <si>
+    <t>Movimientos "drag and drop" del juego.</t>
+  </si>
+  <si>
+    <t>La animación del drag and drop funciona con las cartas y de desactiva cuando se finaliza.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muestra una alerta que impide que se coloque la carta cuando la carta no está en el caldero correcto. </t>
+  </si>
+  <si>
+    <t>Presionar el boton de juego.</t>
+  </si>
+  <si>
+    <t>Se valida la activación y una alerta cuando se intente jugar sin mover la carta en el caldero.</t>
+  </si>
+  <si>
+    <t>El sistema no permite continuar sin un nombre.</t>
+  </si>
+  <si>
+    <t>La lista devuelve el objeto jugador en esa posición (desde modo consola).</t>
+  </si>
+  <si>
+    <t>La lista devuelve un mensaje de advertencia según sea el caso, la posición no es válida o la lista está vacía (desde modo consola).</t>
+  </si>
+  <si>
+    <t>Todos los jugadores se quedan sin cartas al mismo tiempo.</t>
+  </si>
+  <si>
+    <t>Llama a ver ronda en medio del juego.</t>
+  </si>
+  <si>
+    <t>Llamar la función redo, sin haber realizado un undo.</t>
+  </si>
+  <si>
+    <t>Se muestran los resultados hasta ese momento de cada jugador.</t>
+  </si>
+  <si>
+    <t>Se termina una ronda.</t>
+  </si>
+  <si>
+    <t>Muestra una pantalla con los resultados de la ronda.</t>
+  </si>
+  <si>
+    <t>Se come un caldero que contiene venenos.</t>
+  </si>
+  <si>
+    <t>No se podruce ningún cambio.</t>
+  </si>
+  <si>
+    <t>Se añaden estas cartas venenos a la del jugador.</t>
+  </si>
+  <si>
+    <t>Devuelve al movimiento anterior.</t>
+  </si>
+  <si>
+    <t>Vuelve a hacer el movimiento que el undo quitó.</t>
+  </si>
+  <si>
+    <t>No se relaiza ningún cambio.</t>
+  </si>
+  <si>
+    <t>Devuelve la ronda al principio</t>
   </si>
 </sst>
 </file>
@@ -369,7 +385,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -377,11 +393,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -396,9 +523,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -407,11 +531,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -444,21 +595,6 @@
           <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -504,6 +640,37 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="admin" refreshedDate="42844.735411805559" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="50">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Tabla1"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Id " numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="50"/>
+    </cacheField>
+    <cacheField name="Descripción" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Resultado esperado" numFmtId="0">
+      <sharedItems containsBlank="1" longText="1"/>
+    </cacheField>
+    <cacheField name="Estado" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Certificado"/>
+        <s v="Pendiente"/>
+        <s v="Con Error"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="50">
   <r>
@@ -809,9 +976,314 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="50">
+  <r>
+    <n v="1"/>
+    <s v="Al iniciar el juego se abre correctamente el socket."/>
+    <s v="Se ejecute background en un proceso de Windows."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="Al presionar el ejecutable se ejecuta el apache y las dependencias."/>
+    <s v="Al iniciar se ejecute como aplicación secundaria el módulo apache y sus dependencias, sin que el usuario lo observe."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <s v="Iniciar el juego."/>
+    <s v="Al iniciar se abre correctamente el explorador por defecto y se inicia la animacion principal."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <s v="Enlace al manual de usuario. "/>
+    <s v="Cada pantalla con un enlace al manual de usuario, y que este este correctamente enlazado."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <s v="En todas las pantallas de juego existe un enlace a atrás validando en los casos en los que no pueda ir, como al inciar la consola de juego. "/>
+    <s v="Enlaces de atrás correctamente validados alas pantallas correspondientes"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <s v="Movimientos &quot;drag and drop&quot; del juego."/>
+    <s v="La animación del drag and drop funciona con las cartas y de desactiva cuando se finaliza."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <s v="Se valida la carta con la UI en el caldero y verifica que la carta pueda o no colocarse en el caldero"/>
+    <s v="Muestra una alerta que impide que se coloque la carta cuando la carta no está en el caldero correcto. "/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <s v="Presionar el boton de juego."/>
+    <s v="Se valida la activación y una alerta cuando se intente jugar sin mover la carta en el caldero."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <s v="Asignar la cantidad de jugadores en uno."/>
+    <s v="No se puede crear solo un jugador, el mínimo son dos."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <s v="Asignar la cantidad de jugadores en dos."/>
+    <s v="La cantidad es aceptada correctamente."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <s v="Asignar la cantidad de jugadores en siete."/>
+    <s v="No es posible, el máximo son seis jugadores."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <s v="No digita el nombre del jugador al crearlo."/>
+    <s v="El sistema no permite continuar sin un nombre."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <s v="Digita un nombre al jugador al crearlo."/>
+    <s v="Se le asigna el string digitado como nombre al guardar el jugador en la lista."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <s v="Se crean seis jugadores, se les asigna un nombre a cada uno."/>
+    <s v="La lista de jugadores debe contener 6 jugadores, cada uno con el nombre asignado, y un id que indica el orden en que fueron creados."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <s v="Busca un jugador según su posición en la lista (la posición existe)."/>
+    <s v="La lista devuelve el objeto jugador en esa posición (desde modo consola)."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <s v="Busca un jugador según su posición en la lista (la posición no existe)."/>
+    <s v="La lista devuelve un mensaje de advertencia según sea el caso, la posición no es válida o la lista está vacía (desde modo consola)."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <s v="Busca la baraja de cartas en mano de un jugador en específico."/>
+    <s v="Devuelve la baraja  de cartas en mano, o un mensaje de advertencia en caso de que esta esté vacía."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <s v="Busca la baraja de cartas  comidas de un jugador en específico."/>
+    <s v="Devuelve la baraja  de cartas comidas, o un mensaje de advertencia en caso de que esta esté vacía."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <s v="Busca la baraja de cartas veneno de un jugador en específico."/>
+    <s v="Devuelve la baraja  de cartas veneno, o un mensaje de advertencia en caso de que esta esté vacía."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="20"/>
+    <s v="Llama a la opción barajar antes de empezar la ronda."/>
+    <s v="Se reparte una cantidad de cartas cada jugador según la cantidad de jugadores activos, estas cartas son repartidas de manera aleatoria."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="21"/>
+    <s v="Después de barajar  se consulta el pozo para repartir."/>
+    <s v="Devuelve el pozo, este debe ser el pozo original, menos las cartas previamente repartidas."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <s v="Llama a la opción barajar, mientras algún jugador todavía tiene cartas."/>
+    <s v="Sólo se puede barajar cuando todos los jugadores no tengan ninguna carta en la mano."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="23"/>
+    <s v="Llama a la opción barajar (en el pozo no quedan suficientes cartas para repartir según las reglas)"/>
+    <s v="Se termina la ronda."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <s v="Se añade una carta (que no es veneno) a un caldero vacío."/>
+    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <s v="Se añade una carta (que no es veneno) a un caldero no vacío, pero que tiene la misma nomenclatura. El total del caldero es menor que trece."/>
+    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <s v="Se añade una carta (que no es veneno) a un caldero con diferente nomenclatura."/>
+    <s v="El sistema rechaza el movimiento."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <s v="Se añade una carta (que no es veneno) a un caldero. El total del caldero da más de trece."/>
+    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador. Al verificar el total, da mayor de lo establecido, por lo cual las cartas en el caldero se pasan a la baraja de cartas comidas por el jugador. Admás si entre estas existen cartas venenos estas se pasan a la baraja de cartas veneno del jugador."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <s v="Se añade una carta veneno a un caldero no vacío. El total del caldero es menor que trece."/>
+    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <s v="Se añade una carta veneno a un caldero vacío. El jugador tiene más cartas en la mano."/>
+    <s v="Se rechaza el movimiento."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="30"/>
+    <s v="Se añade una carta veneno a un caldero vacío. El jugador sólo tiene esa carta en la mano."/>
+    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="31"/>
+    <s v="Se añade una carta veneno a un caldero que contiene solamente cartas veneno.  El jugador sólo tiene esa carta en la mano."/>
+    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <s v="Se añade una carta veneno a un caldero que contiene solamente cartas veneno.  El jugador tiene más cartas en la mano."/>
+    <s v="El sistema rechaza el movimiento."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="33"/>
+    <s v="Se añade una carta veneno a un caldero. El total del caldero da más de trece."/>
+    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador. Al verificar el total, da mayor de lo establecido, por lo cual las cartas en el caldero se pasan a la baraja de cartas comidas por el jugador. Admás si entre estas existen cartas venenos estas se pasan a la baraja de cartas veneno del jugador."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="34"/>
+    <s v="Pasar de turno sin haber añadido a algún caldero. El jugador tiene cartas en la mano."/>
+    <s v="El sistema no permite continuar con el juego hasta que el jugador en el turno mueva la carta."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="35"/>
+    <s v="Pasar de turno sin haber añadido a algún caldero. El jugador no tiene cartas."/>
+    <s v="Todos los jugadores se quedan sin cartas al mismo tiempo."/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="36"/>
+    <s v="Llama a ver ronda en medio del juego."/>
+    <s v="Se muestran los resultados hasta ese momento de cada jugador."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="37"/>
+    <s v="Se termina una ronda."/>
+    <s v="Muestra una pantalla con los resultados de la ronda."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="38"/>
+    <s v="Se come un caldero que contiene venenos."/>
+    <s v="Se añaden estas cartas venenos a la del jugador."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="40"/>
+    <s v="Llamar la función undo, en medio de una ronda."/>
+    <s v="Devuelve al movimiento anterior."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="41"/>
+    <s v="Llamar la función redo, sin haber realizado un undo."/>
+    <s v="No se podruce ningún cambio."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="42"/>
+    <s v="Llamar la función redo, después de un undo."/>
+    <s v="Vuelve a hacer el movimiento que el undo quitó."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="43"/>
+    <s v="Llamar la función reset al empezar una ronda."/>
+    <s v="No se relaiza ningún cambio."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="44"/>
+    <s v="Llamar la función reset en medio de una ronda."/>
+    <s v="Devuelve la ronda al principio"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="45"/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="46"/>
+    <s v="Se acaban las cartas en el pozo de repartir. Un jugador no tiene ninguna carta veneno."/>
+    <s v="Se acaba la ronda y dicho jugador sale del juego."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="47"/>
+    <s v="Se acaban las cartas en el pozo de repartir. Ningún jugador tiene cartas veneno."/>
+    <s v="Se acaba el juego."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="48"/>
+    <s v="Se acaban las cartas en el pozo de repartir. Todos los jugadores tienen la misma cantidad de cartas venenos."/>
+    <s v="Se acaba el juego."/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="49"/>
+    <s v="Se acaban las cartas en el pozo para repartir. Varios jugadores tienen la misma cantidad de venenos."/>
+    <s v="Se crea una neva ronda, y se sacan del juego los jugadores que tengan menor cantidad de venenos."/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="50"/>
+    <s v="Se acaban las cartas en el pozo para repartir. Sólo quedan dos jugadores."/>
+    <s v="Se saca el jugador con menos cartas venenos, el otro es el perdedor."/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B62:C66" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -860,14 +1332,42 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="">
+  <location ref="B62:D79" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="4">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B4:E54" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B4:E54" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="B4:E54"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Id " dataDxfId="6"/>
-    <tableColumn id="2" name="Descripción" dataDxfId="5"/>
-    <tableColumn id="3" name="Resultado esperado" dataDxfId="4"/>
-    <tableColumn id="4" name="Estado" dataDxfId="3"/>
+    <tableColumn id="1" name="Id " dataDxfId="3"/>
+    <tableColumn id="2" name="Descripción" dataDxfId="2"/>
+    <tableColumn id="3" name="Resultado esperado" dataDxfId="1"/>
+    <tableColumn id="4" name="Estado" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1170,10 +1670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A3:B7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,33 +1681,75 @@
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="8">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G66"/>
+  <dimension ref="B2:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60:C60"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="4" max="4" width="52.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" customWidth="1"/>
+    <col min="4" max="4" width="61.140625" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
@@ -1236,10 +1778,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>5</v>
@@ -1253,10 +1795,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>5</v>
@@ -1270,10 +1812,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>5</v>
@@ -1285,10 +1827,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>5</v>
@@ -1299,10 +1841,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>5</v>
@@ -1313,10 +1855,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>5</v>
@@ -1327,10 +1869,10 @@
         <v>7</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>5</v>
@@ -1341,10 +1883,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>5</v>
@@ -1361,7 +1903,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -1375,7 +1917,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -1389,10 +1931,10 @@
         <v>13</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>12</v>
       </c>
@@ -1400,10 +1942,10 @@
         <v>14</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1414,10 +1956,10 @@
         <v>15</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -1425,13 +1967,13 @@
         <v>14</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1439,13 +1981,13 @@
         <v>15</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1453,13 +1995,13 @@
         <v>16</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1467,13 +2009,13 @@
         <v>17</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="E21" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1481,13 +2023,13 @@
         <v>18</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="E22" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1495,13 +2037,13 @@
         <v>19</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="E23" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="45" x14ac:dyDescent="0.25">
@@ -1509,13 +2051,13 @@
         <v>20</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1523,13 +2065,13 @@
         <v>21</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1537,13 +2079,13 @@
         <v>22</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1551,13 +2093,13 @@
         <v>23</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1565,13 +2107,13 @@
         <v>24</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="45" x14ac:dyDescent="0.25">
@@ -1579,13 +2121,13 @@
         <v>25</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1593,13 +2135,13 @@
         <v>26</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="90" x14ac:dyDescent="0.25">
@@ -1607,13 +2149,13 @@
         <v>27</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1621,13 +2163,13 @@
         <v>28</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1635,13 +2177,13 @@
         <v>29</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1649,13 +2191,13 @@
         <v>30</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="45" x14ac:dyDescent="0.25">
@@ -1663,10 +2205,10 @@
         <v>31</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>7</v>
@@ -1677,13 +2219,13 @@
         <v>32</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="90" x14ac:dyDescent="0.25">
@@ -1691,13 +2233,13 @@
         <v>33</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1705,13 +2247,13 @@
         <v>34</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1719,13 +2261,13 @@
         <v>35</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
@@ -1733,9 +2275,11 @@
         <v>36</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D40" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="E40" s="3" t="s">
         <v>7</v>
       </c>
@@ -1745,9 +2289,11 @@
         <v>37</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D41" s="5"/>
+        <v>91</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="E41" s="3" t="s">
         <v>7</v>
       </c>
@@ -1757,9 +2303,11 @@
         <v>38</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D42" s="5"/>
+        <v>93</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="E42" s="3" t="s">
         <v>7</v>
       </c>
@@ -1768,12 +2316,10 @@
       <c r="B43" s="4">
         <v>39</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
@@ -1781,21 +2327,25 @@
         <v>40</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="E44" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="4">
         <v>41</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="E45" s="3" t="s">
         <v>7</v>
       </c>
@@ -1805,9 +2355,11 @@
         <v>42</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="E46" s="3" t="s">
         <v>7</v>
       </c>
@@ -1817,9 +2369,11 @@
         <v>43</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D47" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="E47" s="3" t="s">
         <v>7</v>
       </c>
@@ -1829,9 +2383,11 @@
         <v>44</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="E48" s="3" t="s">
         <v>7</v>
       </c>
@@ -1840,9 +2396,7 @@
       <c r="B49" s="4">
         <v>45</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="3" t="s">
         <v>7</v>
@@ -1853,10 +2407,10 @@
         <v>46</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>7</v>
@@ -1867,10 +2421,10 @@
         <v>47</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>7</v>
@@ -1881,10 +2435,10 @@
         <v>48</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>6</v>
@@ -1895,10 +2449,10 @@
         <v>49</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>7</v>
@@ -1909,74 +2463,121 @@
         <v>50</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C60" s="10"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C62" t="s">
-        <v>93</v>
-      </c>
+      <c r="B62" s="11"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="13"/>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" s="9">
-        <v>8</v>
-      </c>
+      <c r="B63" s="14"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="16"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C64" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" s="9">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C66" s="9">
-        <v>50</v>
-      </c>
+      <c r="B64" s="14"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="16"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="14"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="16"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="14"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="16"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="14"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="16"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="14"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="16"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="14"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="16"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="14"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="16"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="14"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="16"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="14"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="16"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="14"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="16"/>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="14"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="16"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="14"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="16"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="14"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="16"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="14"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="16"/>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="14"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="16"/>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="17"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B60:C60"/>
   </mergeCells>
   <conditionalFormatting sqref="E5:E54">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Con error">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Con error">
       <formula>NOT(ISERROR(SEARCH("Con error",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Pendiente">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Pendiente">
       <formula>NOT(ISERROR(SEARCH("Pendiente",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Certificado">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Certificado">
       <formula>NOT(ISERROR(SEARCH("Certificado",E5)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Casos de prueba final
</commit_message>
<xml_diff>
--- a/Documentación/Casos de prueba.xlsx
+++ b/Documentación/Casos de prueba.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\Veneno\ED-Veneno\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ED-Veneno\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,8 +21,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
-    <pivotCache cacheId="10" r:id="rId4"/>
+    <pivotCache cacheId="6" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="104">
   <si>
     <t>Casos de prueba</t>
   </si>
@@ -329,10 +328,22 @@
     <t>Vuelve a hacer el movimiento que el undo quitó.</t>
   </si>
   <si>
-    <t>No se relaiza ningún cambio.</t>
-  </si>
-  <si>
     <t>Devuelve la ronda al principio</t>
+  </si>
+  <si>
+    <t>No se realiza ningún cambio.</t>
+  </si>
+  <si>
+    <t>Al ejecutar el juego se abra automáticamente el socket.</t>
+  </si>
+  <si>
+    <t>Se abre el socket y despliega el menú del juego.</t>
+  </si>
+  <si>
+    <t>Mientras se ejecuta una acción en el servidor no se modifque la interfaz.</t>
+  </si>
+  <si>
+    <t>Muestra en pantalla un ícono que indica que se está cargando.</t>
   </si>
 </sst>
 </file>
@@ -385,7 +396,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -393,122 +404,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF999999"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF999999"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="65"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF999999"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="65"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF999999"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF999999"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF999999"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="65"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="65"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="65"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="65"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF999999"/>
-      </right>
-      <top style="thin">
-        <color indexed="65"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF999999"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="65"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF999999"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="65"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="65"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF999999"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="65"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF999999"/>
-      </right>
-      <top style="thin">
-        <color indexed="65"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF999999"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -534,35 +434,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -596,6 +472,21 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -610,7 +501,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="15" refreshedDate="42844.490463310183" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="50">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="15" refreshedDate="42844.950372685184" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="50">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabla1"/>
   </cacheSource>
@@ -622,43 +513,11 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="Resultado esperado" numFmtId="0">
-      <sharedItems containsBlank="1" longText="1"/>
+      <sharedItems longText="1"/>
     </cacheField>
     <cacheField name="Estado" numFmtId="0">
-      <sharedItems count="3">
+      <sharedItems count="2">
         <s v="Certificado"/>
-        <s v="Pendiente"/>
-        <s v="Con Error"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="admin" refreshedDate="42844.735411805559" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="50">
-  <cacheSource type="worksheet">
-    <worksheetSource name="Tabla1"/>
-  </cacheSource>
-  <cacheFields count="4">
-    <cacheField name="Id " numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="50"/>
-    </cacheField>
-    <cacheField name="Descripción" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Resultado esperado" numFmtId="0">
-      <sharedItems containsBlank="1" longText="1"/>
-    </cacheField>
-    <cacheField name="Estado" numFmtId="0">
-      <sharedItems count="3">
-        <s v="Certificado"/>
-        <s v="Pendiente"/>
         <s v="Con Error"/>
       </sharedItems>
     </cacheField>
@@ -681,177 +540,177 @@
   </r>
   <r>
     <n v="2"/>
-    <s v="Al precionar el ejecutable se ejecuta el apache y las dependencias."/>
-    <s v="Al iniciar se ejecute como aplicación secundaria el modulo apache y sus dependencias, sin que el usuario lo observe."/>
+    <s v="Al presionar el ejecutable se ejecuta el apache y las dependencias."/>
+    <s v="Al iniciar se ejecute como aplicación secundaria el módulo apache y sus dependencias, sin que el usuario lo observe."/>
     <x v="0"/>
   </r>
   <r>
     <n v="3"/>
-    <s v="Al abrir se abre correctamente el index e inicia la animacion principal."/>
+    <s v="Iniciar el juego."/>
     <s v="Al iniciar se abre correctamente el explorador por defecto y se inicia la animacion principal."/>
     <x v="0"/>
   </r>
   <r>
     <n v="4"/>
-    <s v="En todas las pantallas de juego existe el enlace al manual de usuario. "/>
+    <s v="Enlace al manual de usuario. "/>
     <s v="Cada pantalla con un enlace al manual de usuario, y que este este correctamente enlazado."/>
     <x v="0"/>
   </r>
   <r>
     <n v="5"/>
-    <s v="En todas las pantallas de juego existe un enlace a atraz validando en los casos en los que no pueda ir, como al inciar la consola de juego. "/>
-    <s v="Enlaces de atraz correctamente validados alas pantallas correspondientes"/>
+    <s v="En todas las pantallas de juego existe un enlace a atrás validando en los casos en los que no pueda ir, como al inciar la consola de juego. "/>
+    <s v="Enlaces de atrás correctamente validados alas pantallas correspondientes"/>
     <x v="0"/>
   </r>
   <r>
     <n v="6"/>
-    <s v="El drag and drop del juego."/>
-    <s v="La animacion del drag and drop funciona con las cartas y de desactiva cuando se finaliza."/>
+    <s v="Movimientos &quot;drag and drop&quot; del juego."/>
+    <s v="La animación del drag and drop funciona con las cartas y de desactiva cuando se finaliza."/>
     <x v="0"/>
   </r>
   <r>
     <n v="7"/>
     <s v="Se valida la carta con la UI en el caldero y verifica que la carta pueda o no colocarse en el caldero"/>
-    <s v="Muestra una alerta que impide que se coloque la carta cuando la carta no esta en el caldero correcto. "/>
+    <s v="Muestra una alerta que impide que se coloque la carta cuando la carta no está en el caldero correcto. "/>
     <x v="0"/>
   </r>
   <r>
     <n v="8"/>
-    <s v="Se valida el boton de juego."/>
-    <s v="Se valida la activacion y una alerta cuando se intente jugar sin mover la carta en el caldero."/>
+    <s v="Presionar el boton de juego."/>
+    <s v="Se valida la activación y una alerta cuando se intente jugar sin mover la carta en el caldero."/>
     <x v="0"/>
   </r>
   <r>
     <n v="9"/>
     <s v="Asignar la cantidad de jugadores en uno."/>
     <s v="No se puede crear solo un jugador, el mínimo son dos."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="10"/>
     <s v="Asignar la cantidad de jugadores en dos."/>
     <s v="La cantidad es aceptada correctamente."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="11"/>
     <s v="Asignar la cantidad de jugadores en siete."/>
     <s v="No es posible, el máximo son seis jugadores."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="12"/>
     <s v="No digita el nombre del jugador al crearlo."/>
-    <s v="Se le asigna como nombre &quot;Jugador n&quot;, donde n es el número del jugador."/>
-    <x v="1"/>
+    <s v="El sistema no permite continuar sin un nombre."/>
+    <x v="0"/>
   </r>
   <r>
     <n v="13"/>
     <s v="Digita un nombre al jugador al crearlo."/>
     <s v="Se le asigna el string digitado como nombre al guardar el jugador en la lista."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="14"/>
     <s v="Se crean seis jugadores, se les asigna un nombre a cada uno."/>
     <s v="La lista de jugadores debe contener 6 jugadores, cada uno con el nombre asignado, y un id que indica el orden en que fueron creados."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="15"/>
     <s v="Busca un jugador según su posición en la lista (la posición existe)."/>
-    <s v="La lista devuelve el objeto jugador en esa posición."/>
-    <x v="1"/>
+    <s v="La lista devuelve el objeto jugador en esa posición (desde modo consola)."/>
+    <x v="0"/>
   </r>
   <r>
     <n v="16"/>
     <s v="Busca un jugador según su posición en la lista (la posición no existe)."/>
-    <s v="La lista devuelve un mensaje de advertencia según sea el caso, la posición no es válida o la lista está vacía."/>
-    <x v="1"/>
+    <s v="La lista devuelve un mensaje de advertencia según sea el caso, la posición no es válida o la lista está vacía (desde modo consola)."/>
+    <x v="0"/>
   </r>
   <r>
     <n v="17"/>
     <s v="Busca la baraja de cartas en mano de un jugador en específico."/>
     <s v="Devuelve la baraja  de cartas en mano, o un mensaje de advertencia en caso de que esta esté vacía."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="18"/>
     <s v="Busca la baraja de cartas  comidas de un jugador en específico."/>
     <s v="Devuelve la baraja  de cartas comidas, o un mensaje de advertencia en caso de que esta esté vacía."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="19"/>
     <s v="Busca la baraja de cartas veneno de un jugador en específico."/>
     <s v="Devuelve la baraja  de cartas veneno, o un mensaje de advertencia en caso de que esta esté vacía."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="20"/>
     <s v="Llama a la opción barajar antes de empezar la ronda."/>
     <s v="Se reparte una cantidad de cartas cada jugador según la cantidad de jugadores activos, estas cartas son repartidas de manera aleatoria."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="21"/>
     <s v="Después de barajar  se consulta el pozo para repartir."/>
     <s v="Devuelve el pozo, este debe ser el pozo original, menos las cartas previamente repartidas."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="22"/>
     <s v="Llama a la opción barajar, mientras algún jugador todavía tiene cartas."/>
     <s v="Sólo se puede barajar cuando todos los jugadores no tengan ninguna carta en la mano."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="23"/>
     <s v="Llama a la opción barajar (en el pozo no quedan suficientes cartas para repartir según las reglas)"/>
     <s v="Se termina la ronda."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="24"/>
     <s v="Se añade una carta (que no es veneno) a un caldero vacío."/>
     <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="25"/>
     <s v="Se añade una carta (que no es veneno) a un caldero no vacío, pero que tiene la misma nomenclatura. El total del caldero es menor que trece."/>
     <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="26"/>
     <s v="Se añade una carta (que no es veneno) a un caldero con diferente nomenclatura."/>
     <s v="El sistema rechaza el movimiento."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="27"/>
     <s v="Se añade una carta (que no es veneno) a un caldero. El total del caldero da más de trece."/>
     <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador. Al verificar el total, da mayor de lo establecido, por lo cual las cartas en el caldero se pasan a la baraja de cartas comidas por el jugador. Admás si entre estas existen cartas venenos estas se pasan a la baraja de cartas veneno del jugador."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="28"/>
     <s v="Se añade una carta veneno a un caldero no vacío. El total del caldero es menor que trece."/>
     <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="29"/>
     <s v="Se añade una carta veneno a un caldero vacío. El jugador tiene más cartas en la mano."/>
     <s v="Se rechaza el movimiento."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="30"/>
     <s v="Se añade una carta veneno a un caldero vacío. El jugador sólo tiene esa carta en la mano."/>
     <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="31"/>
@@ -863,109 +722,109 @@
     <n v="32"/>
     <s v="Se añade una carta veneno a un caldero que contiene solamente cartas veneno.  El jugador tiene más cartas en la mano."/>
     <s v="El sistema rechaza el movimiento."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="33"/>
     <s v="Se añade una carta veneno a un caldero. El total del caldero da más de trece."/>
     <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador. Al verificar el total, da mayor de lo establecido, por lo cual las cartas en el caldero se pasan a la baraja de cartas comidas por el jugador. Admás si entre estas existen cartas venenos estas se pasan a la baraja de cartas veneno del jugador."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="34"/>
     <s v="Pasar de turno sin haber añadido a algún caldero. El jugador tiene cartas en la mano."/>
     <s v="El sistema no permite continuar con el juego hasta que el jugador en el turno mueva la carta."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="35"/>
     <s v="Pasar de turno sin haber añadido a algún caldero. El jugador no tiene cartas."/>
-    <s v="Se realiza automáticamente, al jugador que se queda sin cartas se le pasa el turno."/>
+    <s v="Todos los jugadores se quedan sin cartas al mismo tiempo."/>
     <x v="1"/>
   </r>
   <r>
     <n v="36"/>
-    <s v="Llamar la función undo, empezar una ronda."/>
-    <m/>
-    <x v="1"/>
+    <s v="Llama a ver ronda en medio del juego."/>
+    <s v="Se muestran los resultados hasta ese momento de cada jugador."/>
+    <x v="0"/>
   </r>
   <r>
     <n v="37"/>
+    <s v="Se termina una ronda."/>
+    <s v="Muestra una pantalla con los resultados de la ronda."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="38"/>
+    <s v="Se come un caldero que contiene venenos."/>
+    <s v="Se añaden estas cartas venenos a la del jugador."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <s v="Al ejecutar el juego se abra automáticamente el socket."/>
+    <s v="Se abre el socket y despliega el menú del juego."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="40"/>
     <s v="Llamar la función undo, en medio de una ronda."/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="38"/>
-    <s v="Llamar la función undo al finalizar la ronda."/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="39"/>
-    <s v="Llamar la función redo, sin ahaber realizado un undo."/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="40"/>
+    <s v="Devuelve al movimiento anterior."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="41"/>
+    <s v="Llamar la función redo, sin haber realizado un undo."/>
+    <s v="No se podruce ningún cambio."/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="42"/>
     <s v="Llamar la función redo, después de un undo."/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="41"/>
-    <s v="Llamar la función redo, después de un undo, y luego jugar un movimiento"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="42"/>
-    <s v="Llamar la función redo dos veces después de un undo."/>
-    <m/>
+    <s v="Vuelve a hacer el movimiento que el undo quitó."/>
     <x v="1"/>
   </r>
   <r>
     <n v="43"/>
     <s v="Llamar la función reset al empezar una ronda."/>
-    <m/>
-    <x v="1"/>
+    <s v="No se realiza ningún cambio."/>
+    <x v="0"/>
   </r>
   <r>
     <n v="44"/>
     <s v="Llamar la función reset en medio de una ronda."/>
-    <m/>
+    <s v="Devuelve la ronda al principio"/>
     <x v="1"/>
   </r>
   <r>
     <n v="45"/>
-    <s v="Llamar la función reset al finalizar una ronda."/>
-    <m/>
-    <x v="1"/>
+    <s v="Mientras se ejecuta una acción en el servidor no se modifque la interfaz."/>
+    <s v="Muestra en pantalla un ícono que indica que se está cargando."/>
+    <x v="0"/>
   </r>
   <r>
     <n v="46"/>
     <s v="Se acaban las cartas en el pozo de repartir. Un jugador no tiene ninguna carta veneno."/>
     <s v="Se acaba la ronda y dicho jugador sale del juego."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="47"/>
     <s v="Se acaban las cartas en el pozo de repartir. Ningún jugador tiene cartas veneno."/>
     <s v="Se acaba el juego."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="48"/>
     <s v="Se acaban las cartas en el pozo de repartir. Todos los jugadores tienen la misma cantidad de cartas venenos."/>
     <s v="Se acaba el juego."/>
-    <x v="2"/>
+    <x v="1"/>
   </r>
   <r>
     <n v="49"/>
     <s v="Se acaban las cartas en el pozo para repartir. Varios jugadores tienen la misma cantidad de venenos."/>
     <s v="Se crea una neva ronda, y se sacan del juego los jugadores que tengan menor cantidad de venenos."/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="50"/>
@@ -976,322 +835,16 @@
 </pivotCacheRecords>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="50">
-  <r>
-    <n v="1"/>
-    <s v="Al iniciar el juego se abre correctamente el socket."/>
-    <s v="Se ejecute background en un proceso de Windows."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <s v="Al presionar el ejecutable se ejecuta el apache y las dependencias."/>
-    <s v="Al iniciar se ejecute como aplicación secundaria el módulo apache y sus dependencias, sin que el usuario lo observe."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="3"/>
-    <s v="Iniciar el juego."/>
-    <s v="Al iniciar se abre correctamente el explorador por defecto y se inicia la animacion principal."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="4"/>
-    <s v="Enlace al manual de usuario. "/>
-    <s v="Cada pantalla con un enlace al manual de usuario, y que este este correctamente enlazado."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="5"/>
-    <s v="En todas las pantallas de juego existe un enlace a atrás validando en los casos en los que no pueda ir, como al inciar la consola de juego. "/>
-    <s v="Enlaces de atrás correctamente validados alas pantallas correspondientes"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="6"/>
-    <s v="Movimientos &quot;drag and drop&quot; del juego."/>
-    <s v="La animación del drag and drop funciona con las cartas y de desactiva cuando se finaliza."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="7"/>
-    <s v="Se valida la carta con la UI en el caldero y verifica que la carta pueda o no colocarse en el caldero"/>
-    <s v="Muestra una alerta que impide que se coloque la carta cuando la carta no está en el caldero correcto. "/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="8"/>
-    <s v="Presionar el boton de juego."/>
-    <s v="Se valida la activación y una alerta cuando se intente jugar sin mover la carta en el caldero."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="9"/>
-    <s v="Asignar la cantidad de jugadores en uno."/>
-    <s v="No se puede crear solo un jugador, el mínimo son dos."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="10"/>
-    <s v="Asignar la cantidad de jugadores en dos."/>
-    <s v="La cantidad es aceptada correctamente."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="11"/>
-    <s v="Asignar la cantidad de jugadores en siete."/>
-    <s v="No es posible, el máximo son seis jugadores."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="12"/>
-    <s v="No digita el nombre del jugador al crearlo."/>
-    <s v="El sistema no permite continuar sin un nombre."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="13"/>
-    <s v="Digita un nombre al jugador al crearlo."/>
-    <s v="Se le asigna el string digitado como nombre al guardar el jugador en la lista."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="14"/>
-    <s v="Se crean seis jugadores, se les asigna un nombre a cada uno."/>
-    <s v="La lista de jugadores debe contener 6 jugadores, cada uno con el nombre asignado, y un id que indica el orden en que fueron creados."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="15"/>
-    <s v="Busca un jugador según su posición en la lista (la posición existe)."/>
-    <s v="La lista devuelve el objeto jugador en esa posición (desde modo consola)."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="16"/>
-    <s v="Busca un jugador según su posición en la lista (la posición no existe)."/>
-    <s v="La lista devuelve un mensaje de advertencia según sea el caso, la posición no es válida o la lista está vacía (desde modo consola)."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="17"/>
-    <s v="Busca la baraja de cartas en mano de un jugador en específico."/>
-    <s v="Devuelve la baraja  de cartas en mano, o un mensaje de advertencia en caso de que esta esté vacía."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="18"/>
-    <s v="Busca la baraja de cartas  comidas de un jugador en específico."/>
-    <s v="Devuelve la baraja  de cartas comidas, o un mensaje de advertencia en caso de que esta esté vacía."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="19"/>
-    <s v="Busca la baraja de cartas veneno de un jugador en específico."/>
-    <s v="Devuelve la baraja  de cartas veneno, o un mensaje de advertencia en caso de que esta esté vacía."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="20"/>
-    <s v="Llama a la opción barajar antes de empezar la ronda."/>
-    <s v="Se reparte una cantidad de cartas cada jugador según la cantidad de jugadores activos, estas cartas son repartidas de manera aleatoria."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="21"/>
-    <s v="Después de barajar  se consulta el pozo para repartir."/>
-    <s v="Devuelve el pozo, este debe ser el pozo original, menos las cartas previamente repartidas."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="22"/>
-    <s v="Llama a la opción barajar, mientras algún jugador todavía tiene cartas."/>
-    <s v="Sólo se puede barajar cuando todos los jugadores no tengan ninguna carta en la mano."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="23"/>
-    <s v="Llama a la opción barajar (en el pozo no quedan suficientes cartas para repartir según las reglas)"/>
-    <s v="Se termina la ronda."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="24"/>
-    <s v="Se añade una carta (que no es veneno) a un caldero vacío."/>
-    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="25"/>
-    <s v="Se añade una carta (que no es veneno) a un caldero no vacío, pero que tiene la misma nomenclatura. El total del caldero es menor que trece."/>
-    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="26"/>
-    <s v="Se añade una carta (que no es veneno) a un caldero con diferente nomenclatura."/>
-    <s v="El sistema rechaza el movimiento."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="27"/>
-    <s v="Se añade una carta (que no es veneno) a un caldero. El total del caldero da más de trece."/>
-    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador. Al verificar el total, da mayor de lo establecido, por lo cual las cartas en el caldero se pasan a la baraja de cartas comidas por el jugador. Admás si entre estas existen cartas venenos estas se pasan a la baraja de cartas veneno del jugador."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="28"/>
-    <s v="Se añade una carta veneno a un caldero no vacío. El total del caldero es menor que trece."/>
-    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="29"/>
-    <s v="Se añade una carta veneno a un caldero vacío. El jugador tiene más cartas en la mano."/>
-    <s v="Se rechaza el movimiento."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="30"/>
-    <s v="Se añade una carta veneno a un caldero vacío. El jugador sólo tiene esa carta en la mano."/>
-    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="31"/>
-    <s v="Se añade una carta veneno a un caldero que contiene solamente cartas veneno.  El jugador sólo tiene esa carta en la mano."/>
-    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="32"/>
-    <s v="Se añade una carta veneno a un caldero que contiene solamente cartas veneno.  El jugador tiene más cartas en la mano."/>
-    <s v="El sistema rechaza el movimiento."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="33"/>
-    <s v="Se añade una carta veneno a un caldero. El total del caldero da más de trece."/>
-    <s v="Se añade la carta al arreglo del caldero, y se borra de la mano del jugador. Al verificar el total, da mayor de lo establecido, por lo cual las cartas en el caldero se pasan a la baraja de cartas comidas por el jugador. Admás si entre estas existen cartas venenos estas se pasan a la baraja de cartas veneno del jugador."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="34"/>
-    <s v="Pasar de turno sin haber añadido a algún caldero. El jugador tiene cartas en la mano."/>
-    <s v="El sistema no permite continuar con el juego hasta que el jugador en el turno mueva la carta."/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="35"/>
-    <s v="Pasar de turno sin haber añadido a algún caldero. El jugador no tiene cartas."/>
-    <s v="Todos los jugadores se quedan sin cartas al mismo tiempo."/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="36"/>
-    <s v="Llama a ver ronda en medio del juego."/>
-    <s v="Se muestran los resultados hasta ese momento de cada jugador."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="37"/>
-    <s v="Se termina una ronda."/>
-    <s v="Muestra una pantalla con los resultados de la ronda."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="38"/>
-    <s v="Se come un caldero que contiene venenos."/>
-    <s v="Se añaden estas cartas venenos a la del jugador."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="39"/>
-    <m/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="40"/>
-    <s v="Llamar la función undo, en medio de una ronda."/>
-    <s v="Devuelve al movimiento anterior."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="41"/>
-    <s v="Llamar la función redo, sin haber realizado un undo."/>
-    <s v="No se podruce ningún cambio."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="42"/>
-    <s v="Llamar la función redo, después de un undo."/>
-    <s v="Vuelve a hacer el movimiento que el undo quitó."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="43"/>
-    <s v="Llamar la función reset al empezar una ronda."/>
-    <s v="No se relaiza ningún cambio."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="44"/>
-    <s v="Llamar la función reset en medio de una ronda."/>
-    <s v="Devuelve la ronda al principio"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="45"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="46"/>
-    <s v="Se acaban las cartas en el pozo de repartir. Un jugador no tiene ninguna carta veneno."/>
-    <s v="Se acaba la ronda y dicho jugador sale del juego."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="47"/>
-    <s v="Se acaban las cartas en el pozo de repartir. Ningún jugador tiene cartas veneno."/>
-    <s v="Se acaba el juego."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="48"/>
-    <s v="Se acaban las cartas en el pozo de repartir. Todos los jugadores tienen la misma cantidad de cartas venenos."/>
-    <s v="Se acaba el juego."/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="49"/>
-    <s v="Se acaban las cartas en el pozo para repartir. Varios jugadores tienen la misma cantidad de venenos."/>
-    <s v="Se crea una neva ronda, y se sacan del juego los jugadores que tengan menor cantidad de venenos."/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="50"/>
-    <s v="Se acaban las cartas en el pozo para repartir. Sólo quedan dos jugadores."/>
-    <s v="Se saca el jugador con menos cartas venenos, el otro es el perdedor."/>
-    <x v="1"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="4">
+      <items count="3">
         <item x="0"/>
-        <item x="2"/>
         <item x="1"/>
         <item t="default"/>
       </items>
@@ -1300,15 +853,12 @@
   <rowFields count="1">
     <field x="3"/>
   </rowFields>
-  <rowItems count="4">
+  <rowItems count="3">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
     </i>
     <i t="grand">
       <x/>
@@ -1332,42 +882,14 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="">
-  <location ref="B62:D79" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="4">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B4:E54" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B4:E54" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="B4:E54"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Id " dataDxfId="3"/>
-    <tableColumn id="2" name="Descripción" dataDxfId="2"/>
-    <tableColumn id="3" name="Resultado esperado" dataDxfId="1"/>
-    <tableColumn id="4" name="Estado" dataDxfId="0"/>
+    <tableColumn id="1" name="Id " dataDxfId="6"/>
+    <tableColumn id="2" name="Descripción" dataDxfId="5"/>
+    <tableColumn id="3" name="Resultado esperado" dataDxfId="4"/>
+    <tableColumn id="4" name="Estado" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1670,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B7"/>
+  <dimension ref="A3:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C9" sqref="A3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1695,7 +1217,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1703,22 +1225,14 @@
         <v>6</v>
       </c>
       <c r="B5" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B6" s="8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="8">
         <v>50</v>
       </c>
     </row>
@@ -1729,16 +1243,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G79"/>
+  <dimension ref="B2:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E54" sqref="B4:E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" customWidth="1"/>
+    <col min="3" max="3" width="77.7109375" customWidth="1"/>
     <col min="4" max="4" width="61.140625" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
   </cols>
@@ -1790,7 +1304,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>2</v>
       </c>
@@ -1836,7 +1350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>5</v>
       </c>
@@ -2144,7 +1658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>27</v>
       </c>
@@ -2200,7 +1714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="4">
         <v>31</v>
       </c>
@@ -2211,10 +1725,10 @@
         <v>36</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="4">
         <v>32</v>
       </c>
@@ -2228,7 +1742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B37" s="4">
         <v>33</v>
       </c>
@@ -2281,7 +1795,7 @@
         <v>90</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
@@ -2295,7 +1809,7 @@
         <v>92</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
@@ -2309,15 +1823,19 @@
         <v>95</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="4">
         <v>39</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+      <c r="C43" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="E43" s="3" t="s">
         <v>5</v>
       </c>
@@ -2333,7 +1851,7 @@
         <v>96</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
@@ -2347,7 +1865,7 @@
         <v>94</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
@@ -2361,7 +1879,7 @@
         <v>97</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
@@ -2372,10 +1890,10 @@
         <v>54</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
@@ -2386,20 +1904,24 @@
         <v>55</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B49" s="4">
         <v>45</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="C49" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="E49" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -2413,7 +1935,7 @@
         <v>57</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -2427,7 +1949,7 @@
         <v>59</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -2455,7 +1977,7 @@
         <v>62</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -2469,127 +1991,37 @@
         <v>64</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="11"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="13"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="14"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="16"/>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="14"/>
-      <c r="C64" s="15"/>
-      <c r="D64" s="16"/>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="14"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="16"/>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="14"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="16"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="14"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="16"/>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="14"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="16"/>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="14"/>
-      <c r="C69" s="15"/>
-      <c r="D69" s="16"/>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="14"/>
-      <c r="C70" s="15"/>
-      <c r="D70" s="16"/>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="14"/>
-      <c r="C71" s="15"/>
-      <c r="D71" s="16"/>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="14"/>
-      <c r="C72" s="15"/>
-      <c r="D72" s="16"/>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="14"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="16"/>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="14"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="16"/>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="14"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="16"/>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="14"/>
-      <c r="C76" s="15"/>
-      <c r="D76" s="16"/>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="14"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="16"/>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="14"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="16"/>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="17"/>
-      <c r="C79" s="18"/>
-      <c r="D79" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="E5:E54">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Con error">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Con error">
       <formula>NOT(ISERROR(SEARCH("Con error",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Pendiente">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Pendiente">
       <formula>NOT(ISERROR(SEARCH("Pendiente",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Certificado">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Certificado">
       <formula>NOT(ISERROR(SEARCH("Certificado",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E53">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E54">
       <formula1>Estado</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>